<commit_message>
Changed C task file to TournamentInfo
</commit_message>
<xml_diff>
--- a/MaintainProjectTasks.xlsx
+++ b/MaintainProjectTasks.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmitc\CS225-March-Madness\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Bug Fixes" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Features" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Improvements" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Bug Fixes" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Improvements" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,18 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
-  <si>
-    <t xml:space="preserve">Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Who</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which files are touched</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>Which files are touched</t>
   </si>
   <si>
     <r>
@@ -54,27 +58,27 @@
         <family val="4"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">If you leave user and password blank and click the login button it creates a user.</t>
+      <t>If you leave user and password blank and click the login button it creates a user.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana Gorohovschi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarchMadnessGUI.java
+    <t>A</t>
+  </si>
+  <si>
+    <t>Ana Gorohovschi</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI.java
 SerializeTest.java</t>
   </si>
   <si>
     <t xml:space="preserve">Trouble finalizing. Is it related to Villanova? </t>
   </si>
   <si>
-    <t xml:space="preserve">Martin&amp;Daniel&amp;Christian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resetSubtree() in Bracket.java</t>
+    <t>Martin&amp;Daniel&amp;Christian</t>
+  </si>
+  <si>
+    <t>resetSubtree() in Bracket.java</t>
   </si>
   <si>
     <r>
@@ -95,20 +99,20 @@
         <family val="4"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Clicking the clear button potentially allow a team to both be eliminated and win.                                                                          a.    Clicking clear while in a region does not clear the final teams.</t>
+      <t>Clicking the clear button potentially allow a team to both be eliminated and win.                                                                          a.    Clicking clear while in a region does not clear the final teams.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Mike S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BracketPane.java</t>
+    <t>Mike S.</t>
+  </si>
+  <si>
+    <t>BracketPane.java</t>
   </si>
   <si>
     <t xml:space="preserve">Error when finalizing “null.ser(access denied)”. </t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t>B</t>
   </si>
   <si>
     <r>
@@ -129,71 +133,71 @@
         <family val="4"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Clear button in FULL region clears only the EAST division.</t>
+      <t>Clear button in FULL region clears only the EAST division.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Benjamin &amp; Ana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bracket.java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once the simulation has been completed, user can’t log out?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vrej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarchMadnessGUI.java</t>
+    <t>Benjamin &amp; Ana</t>
+  </si>
+  <si>
+    <t>Bracket.java</t>
+  </si>
+  <si>
+    <t>Once the simulation has been completed, user can’t log out?</t>
+  </si>
+  <si>
+    <t>Vrej</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI.java</t>
   </si>
   <si>
     <t xml:space="preserve">The user can change a finalize bracket (user can cheat!). </t>
   </si>
   <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Bug not replicable</t>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Note: Bug not replicable</t>
   </si>
   <si>
     <t xml:space="preserve">The system allows the user to create unlimited users. </t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t>C</t>
   </si>
   <si>
     <t xml:space="preserve">Add password encryption. </t>
   </si>
   <si>
-    <t xml:space="preserve">Peter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarchMadnessGUI, Bracket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove user accounts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarchMadnessGUI</t>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI, Bracket</t>
+  </si>
+  <si>
+    <t>Remove user accounts.</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>MarchMadnessGUI</t>
   </si>
   <si>
     <t xml:space="preserve">Add color. </t>
   </si>
   <si>
-    <t xml:space="preserve">Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BracketPane, MarchMadnessGUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resize the full bracket without side scrolling.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thien</t>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>BracketPane, MarchMadnessGUI</t>
+  </si>
+  <si>
+    <t>Resize the full bracket without side scrolling.</t>
+  </si>
+  <si>
+    <t>Thien</t>
   </si>
   <si>
     <t xml:space="preserve">Add seed numbers to brackets. </t>
@@ -202,7 +206,7 @@
     <t xml:space="preserve">Add minimum password length. </t>
   </si>
   <si>
-    <t xml:space="preserve">Nikolas</t>
+    <t>Nikolas</t>
   </si>
   <si>
     <r>
@@ -213,7 +217,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">  </t>
+      <t>  </t>
     </r>
     <r>
       <rPr>
@@ -252,31 +256,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement the simple tutorial. This can be helpful for checking the teams states</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Devin/Paul</t>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Uml</t>
+  </si>
+  <si>
+    <t>Implement the simple tutorial. This can be helpful for checking the teams states</t>
+  </si>
+  <si>
+    <t>Devin/Paul</t>
   </si>
   <si>
     <t xml:space="preserve">Add a warning confirmation dialog when the user is about to finalize.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Gennadiy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MarchmadnessGUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resize (Northern Kentucky, South Dakota State)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">initialmatches.txt, teaminfo.txt</t>
+    <t>Gennadiy</t>
+  </si>
+  <si>
+    <t>MarchmadnessGUI</t>
+  </si>
+  <si>
+    <t>Resize (Northern Kentucky, South Dakota State)</t>
+  </si>
+  <si>
+    <t>initialmatches.txt, teaminfo.txt</t>
   </si>
   <si>
     <r>
@@ -301,35 +305,35 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Change orientation of choose division buttons.</t>
+    <t>Change orientation of choose division buttons.</t>
   </si>
   <si>
     <t xml:space="preserve">Bracketpane  </t>
   </si>
   <si>
-    <t xml:space="preserve">Final two teams should be on top of the platform.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BracketPane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place buttons in one area (drop dpwn menu for the users instead of button)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome message on startup</t>
+    <t>Final two teams should be on top of the platform.</t>
+  </si>
+  <si>
+    <t>BracketPane</t>
+  </si>
+  <si>
+    <t>Place buttons in one area (drop dpwn menu for the users instead of button)</t>
+  </si>
+  <si>
+    <t>Welcome message on startup</t>
   </si>
   <si>
     <t xml:space="preserve">“user winning teams” selection for the simulation board </t>
+  </si>
+  <si>
+    <t>TournamentInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -338,25 +342,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
@@ -394,116 +380,72 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -562,33 +504,341 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
+    <col min="1" max="1" width="87" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,7 +852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -616,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -630,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="59.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -644,13 +894,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -660,7 +910,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -674,7 +924,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
@@ -688,7 +938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
@@ -701,17 +951,17 @@
       <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>25</v>
       </c>
@@ -722,37 +972,29 @@
       <c r="D11" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.71"/>
+    <col min="1" max="1" width="65.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -766,114 +1008,106 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>32</v>
+      <c r="D8" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="89.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.71"/>
+    <col min="1" max="1" width="89.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -887,72 +1121,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
     </row>
-    <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -963,36 +1197,36 @@
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1002,51 +1236,46 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>